<commit_message>
Support case insensitive lookup on Column C (regions)
</commit_message>
<xml_diff>
--- a/tests/data/entry-with-different-words.xlsx
+++ b/tests/data/entry-with-different-words.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t xml:space="preserve">A/ Entrada léxica</t>
   </si>
@@ -37,19 +37,25 @@
     <t xml:space="preserve">E/ Castellano estándar</t>
   </si>
   <si>
-    <t xml:space="preserve">caldereta</t>
+    <t xml:space="preserve">escoba</t>
   </si>
   <si>
     <t xml:space="preserve">s. f. </t>
   </si>
   <si>
-    <t xml:space="preserve">La Pobla de Roda, Torrevelilla, La Ginebrosa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">galleda (del pou)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cubo</t>
+    <t xml:space="preserve">Sopeira</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escombra </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sopeira, Tolba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">escombra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">balea</t>
   </si>
 </sst>
 </file>
@@ -59,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -86,6 +92,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -176,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -202,6 +215,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -285,15 +302,15 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:E8"/>
+      <selection pane="topLeft" activeCell="B56" activeCellId="0" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.14"/>
   </cols>
   <sheetData>
@@ -328,50 +345,60 @@
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>